<commit_message>
Remove table based on feedback
</commit_message>
<xml_diff>
--- a/assignment-1/part-3-table-examples/all.xlsx
+++ b/assignment-1/part-3-table-examples/all.xlsx
@@ -12,7 +12,6 @@
     <sheet name="inventory" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="customers" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="sales" sheetId="4" state="visible" r:id="rId5"/>
-    <sheet name="customer_leads" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -24,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="86">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -149,6 +148,9 @@
     <t xml:space="preserve">country</t>
   </si>
   <si>
+    <t xml:space="preserve">note</t>
+  </si>
+  <si>
     <t xml:space="preserve">Potter</t>
   </si>
   <si>
@@ -188,6 +190,9 @@
     <t xml:space="preserve">190 Clemton Ave</t>
   </si>
   <si>
+    <t xml:space="preserve">Needs loan</t>
+  </si>
+  <si>
     <t xml:space="preserve">Malfoy</t>
   </si>
   <si>
@@ -224,6 +229,9 @@
     <t xml:space="preserve">IN</t>
   </si>
   <si>
+    <t xml:space="preserve">Needs financing</t>
+  </si>
+  <si>
     <t xml:space="preserve">Weasley</t>
   </si>
   <si>
@@ -239,6 +247,9 @@
     <t xml:space="preserve">Champaign</t>
   </si>
   <si>
+    <t xml:space="preserve">Inquiry into financing options</t>
+  </si>
+  <si>
     <t xml:space="preserve">customer_id</t>
   </si>
   <si>
@@ -270,18 +281,6 @@
   </si>
   <si>
     <t xml:space="preserve">10/9/2019</t>
-  </si>
-  <si>
-    <t xml:space="preserve">note</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Needs loan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Needs financing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Inquiry into financing options</t>
   </si>
 </sst>
 </file>
@@ -299,6 +298,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -358,11 +358,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -392,25 +388,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+      <selection pane="topLeft" activeCell="F58" activeCellId="0" sqref="F58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="2.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.03"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="12.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="14.03"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="17.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="7.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="17.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="7.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="25.84"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="19.86"/>
   </cols>
@@ -543,7 +539,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -553,9 +549,9 @@
       <selection pane="topLeft" activeCell="E6" activeCellId="0" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="27.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="27.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="12.37"/>
   </cols>
   <sheetData>
@@ -586,10 +582,10 @@
       <c r="C2" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="D2" s="1" t="n">
+      <c r="D2" s="0" t="n">
         <v>23100</v>
       </c>
-      <c r="E2" s="2" t="n">
+      <c r="E2" s="1" t="n">
         <v>37185</v>
       </c>
     </row>
@@ -603,10 +599,10 @@
       <c r="C3" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="1" t="n">
+      <c r="D3" s="0" t="n">
         <v>35240</v>
       </c>
-      <c r="E3" s="2" t="n">
+      <c r="E3" s="1" t="n">
         <v>37176</v>
       </c>
     </row>
@@ -620,45 +616,38 @@
       <c r="C4" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="D4" s="1" t="n">
+      <c r="D4" s="0" t="n">
         <v>133000</v>
       </c>
-      <c r="E4" s="2" t="n">
+      <c r="E4" s="1" t="n">
         <v>43477</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D5" s="1"/>
-      <c r="E5" s="2"/>
+      <c r="E5" s="1"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D6" s="1"/>
-      <c r="E6" s="2"/>
+      <c r="E6" s="1"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D7" s="1"/>
-      <c r="E7" s="2"/>
+      <c r="E7" s="1"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D8" s="1"/>
-      <c r="E8" s="2"/>
+      <c r="E8" s="1"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D9" s="1"/>
-      <c r="E9" s="2"/>
+      <c r="E9" s="1"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D10" s="1"/>
-      <c r="E10" s="2"/>
+      <c r="E10" s="1"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D11" s="1"/>
-      <c r="E11" s="2"/>
+      <c r="E11" s="1"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -667,17 +656,17 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E6" activeCellId="0" sqref="E6"/>
+      <selection pane="topLeft" activeCell="J6" activeCellId="0" sqref="J6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.94"/>
@@ -715,34 +704,37 @@
       <c r="I1" s="0" t="s">
         <v>40</v>
       </c>
+      <c r="J1" s="0" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -750,25 +742,28 @@
         <v>2</v>
       </c>
       <c r="B3" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="H3" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="I3" s="0" t="s">
         <v>49</v>
       </c>
-      <c r="C3" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="E3" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="F3" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="H3" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="I3" s="0" t="s">
-        <v>48</v>
+      <c r="J3" s="0" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -776,28 +771,28 @@
         <v>3</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -805,25 +800,28 @@
         <v>4</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="I5" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
+      </c>
+      <c r="J5" s="0" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -831,31 +829,34 @@
         <v>5</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="I6" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
+      </c>
+      <c r="J6" s="0" t="s">
+        <v>74</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -864,7 +865,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -874,9 +875,9 @@
       <selection pane="topLeft" activeCell="I5" activeCellId="0" sqref="I5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="20.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="16.81"/>
@@ -890,28 +891,28 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>73</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>74</v>
+        <v>77</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>78</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -927,14 +928,14 @@
       <c r="D2" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="E2" s="1" t="n">
+      <c r="E2" s="0" t="n">
         <v>6300</v>
       </c>
       <c r="G2" s="0" t="n">
         <v>126700</v>
       </c>
-      <c r="H2" s="4" t="s">
-        <v>79</v>
+      <c r="H2" s="3" t="s">
+        <v>83</v>
       </c>
       <c r="I2" s="0" t="n">
         <v>0</v>
@@ -954,13 +955,13 @@
         <v>0</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="G3" s="1" t="n">
+        <v>84</v>
+      </c>
+      <c r="G3" s="0" t="n">
         <v>19635</v>
       </c>
-      <c r="H3" s="4" t="s">
-        <v>81</v>
+      <c r="H3" s="3" t="s">
+        <v>85</v>
       </c>
       <c r="I3" s="0" t="n">
         <v>0</v>
@@ -983,78 +984,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:C4"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="27.37"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="C1" s="0" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="B4" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>85</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>